<commit_message>
iets wat het moet doen
</commit_message>
<xml_diff>
--- a/Grootste maatschappij binnen elke staat.xlsx
+++ b/Grootste maatschappij binnen elke staat.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
-  <si>
-    <t xml:space="preserve">State </t>
-  </si>
-  <si>
-    <t>Verzekering</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Alabama</t>
   </si>
@@ -599,420 +593,416 @@
     <col min="2" max="2" style="7" width="34.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A29" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A30" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A32" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A37" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A39" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A40" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A41" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A43" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A44" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A45" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A46" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A47" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A48" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A49" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A50" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A51" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A52" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>